<commit_message>
Updated the sprint backlog on 26/01/21
Added scrum minutes and acceptance criteria
</commit_message>
<xml_diff>
--- a/Sprint 1/Sprint_Backlog/Sprint backlog.xlsx
+++ b/Sprint 1/Sprint_Backlog/Sprint backlog.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="60">
   <si>
     <t>Agile Group 9 - Sprint 1</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>Calum Parsons</t>
+  </si>
+  <si>
+    <t>Initial Velocity = 11</t>
   </si>
   <si>
     <t>Shanna Balfour</t>
@@ -118,21 +121,92 @@
     <t>As a researcher, I want to be able to add any questionnaires I have designed to my application so that they can get approval</t>
   </si>
   <si>
+    <t>If a created questionairre can be attached to an email then accept</t>
+  </si>
+  <si>
+    <t>Shaun, Tim</t>
+  </si>
+  <si>
     <t>Y/N</t>
   </si>
   <si>
     <t>As a researcher, I want to be able to export data from the questionnaire so that the data can be used for analysis.</t>
   </si>
   <si>
+    <t>All of the questionairre responses can be downloaded in an accessible and easily processible format</t>
+  </si>
+  <si>
+    <t>Shanna</t>
+  </si>
+  <si>
     <t>As a stakeholder, I want participants to only have access to questionnaires so that the rest of the experiment is private and safe</t>
   </si>
   <si>
+    <t>When participants log in, they will only have access to questionnaires on their homepage.</t>
+  </si>
+  <si>
+    <t>Laura + Michael</t>
+  </si>
+  <si>
     <t>As a researcher I want to be able to send questionnaires for participants to fill in so I can collect data from users</t>
   </si>
   <si>
+    <t>Researchers are able to send specific questionnaires to specific participants</t>
+  </si>
+  <si>
+    <t>Gina</t>
+  </si>
+  <si>
     <t>As a researcher, I want the ability to create a questionnaire so that they can be sent to users.</t>
   </si>
   <si>
+    <t>Questionnaires can be designed or processed by the program into its own suitable format</t>
+  </si>
+  <si>
+    <t>Ema, Calum</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="14.0"/>
+      </rPr>
+      <t>Other Tasks:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="9.0"/>
+      </rPr>
+      <t xml:space="preserve"> Not Stories, but still need done</t>
+    </r>
+  </si>
+  <si>
+    <t>Done?</t>
+  </si>
+  <si>
+    <t>Definition of Done:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set up database stuff so we can access it! </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -Meets accessibility guidelines
+-Code has been reviewed
+-Meets acceptance test for story
+-Product Owner accepts story</t>
+  </si>
+  <si>
+    <t>Set up a visual studio c# .net application that works on web</t>
+  </si>
+  <si>
+    <t>Ema + Calum + Timothy</t>
+  </si>
+  <si>
     <t>Scrum Minutes</t>
   </si>
   <si>
@@ -155,12 +229,33 @@
   </si>
   <si>
     <t>4 :)   3 :|   1 :(</t>
+  </si>
+  <si>
+    <t>4 Spirits, 1 Mock, 2 Beer</t>
+  </si>
+  <si>
+    <t>- Lots of research done into best way to host the software</t>
+  </si>
+  <si>
+    <t>- undertanding visual studio            - feeling lost with where to start</t>
+  </si>
+  <si>
+    <t>-database setup                             -github setup                            - everyone able to work comfortably</t>
+  </si>
+  <si>
+    <t>mocktail (happy) 
+beer (ok still) 
+spirit (getting bad)
+industrial strength (uh oh)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
+  </numFmts>
   <fonts count="9">
     <font>
       <sz val="10.0"/>
@@ -190,17 +285,20 @@
     </font>
     <font/>
     <font>
-      <b/>
-      <sz val="11.0"/>
+      <sz val="8.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="9.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
     <font>
       <b/>
       <sz val="12.0"/>
       <color theme="1"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
     </font>
   </fonts>
   <fills count="4">
@@ -223,7 +321,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border/>
     <border>
       <left style="thin">
@@ -316,12 +414,28 @@
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="34">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -346,13 +460,16 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="8" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
@@ -372,29 +489,40 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="14" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="15" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="15" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -666,8 +794,11 @@
       </c>
     </row>
     <row r="6">
+      <c r="A6" s="8" t="s">
+        <v>12</v>
+      </c>
       <c r="I6" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J6" s="6" t="s">
         <v>10</v>
@@ -675,7 +806,7 @@
     </row>
     <row r="7">
       <c r="I7" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J7" s="6" t="s">
         <v>10</v>
@@ -683,219 +814,290 @@
     </row>
     <row r="8">
       <c r="I8" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J8" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9">
-      <c r="I9" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="J9" s="9" t="s">
+      <c r="I9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9" s="10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="10" t="s">
-        <v>16</v>
+      <c r="A10" s="11" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="11" t="s">
+      <c r="A11" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="14" t="s">
+      <c r="B11" s="13"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="12"/>
-      <c r="H11" s="14" t="s">
+      <c r="E11" s="13"/>
+      <c r="F11" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="I11" s="14" t="s">
+      <c r="G11" s="13"/>
+      <c r="H11" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="J11" s="15" t="s">
+      <c r="I11" s="15" t="s">
         <v>22</v>
       </c>
+      <c r="J11" s="16" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="12">
-      <c r="C12" s="16"/>
-      <c r="F12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="18"/>
+      <c r="C12" s="17"/>
+      <c r="F12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="19"/>
     </row>
     <row r="13">
-      <c r="A13" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="H13" s="20">
+      <c r="A13" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="21">
         <v>2.0</v>
       </c>
-      <c r="I13" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="J13" s="20" t="s">
-        <v>24</v>
+      <c r="I13" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="J13" s="21" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="H14" s="20">
+      <c r="A14" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14" s="21">
         <v>2.0</v>
       </c>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
     </row>
     <row r="15">
-      <c r="A15" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="H15" s="20">
+      <c r="A15" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15" s="21">
         <v>2.0</v>
       </c>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
     </row>
     <row r="16">
-      <c r="A16" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="H16" s="20">
+      <c r="A16" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H16" s="21">
         <v>2.0</v>
       </c>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
     </row>
     <row r="17">
-      <c r="A17" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="H17" s="20">
+      <c r="A17" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H17" s="21">
         <v>3.0</v>
       </c>
-      <c r="I17" s="21"/>
-      <c r="J17" s="21"/>
+      <c r="I17" s="23"/>
     </row>
     <row r="18">
-      <c r="A18" s="22"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="23"/>
+      <c r="A18" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
+    </row>
+    <row r="19">
+      <c r="I19" s="8" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="20">
-      <c r="A20" s="24" t="s">
-        <v>29</v>
+      <c r="A20" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I20" s="27" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="E21" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="G21" s="26" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="7"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="7"/>
+      <c r="A21" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="24">
-      <c r="A24" s="7"/>
+      <c r="A24" s="28" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="25">
-      <c r="A25" s="7"/>
+      <c r="A25" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="30"/>
+      <c r="E25" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="F25" s="30"/>
+      <c r="G25" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="H25" s="31"/>
     </row>
     <row r="26">
-      <c r="A26" s="7"/>
+      <c r="A26" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="7"/>
     </row>
     <row r="27">
-      <c r="A27" s="7"/>
+      <c r="A27" s="32">
+        <v>44222.0</v>
+      </c>
+      <c r="B27" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="E27" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="G27" s="20" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="28">
-      <c r="A28" s="7"/>
+      <c r="A28" s="32">
+        <v>44223.0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="7"/>
     </row>
+    <row r="37">
+      <c r="I37" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="43">
+  <mergeCells count="46">
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G31:H31"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:C17"/>
     <mergeCell ref="A11:C12"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="D13:E13"/>
     <mergeCell ref="D11:E12"/>
     <mergeCell ref="F11:G12"/>
     <mergeCell ref="H11:H12"/>
     <mergeCell ref="I11:I12"/>
     <mergeCell ref="J11:J12"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="D18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="I20:J23"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="A18:C19"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="A21:C21"/>
     <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
     <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G26:H26"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>